<commit_message>
Fixed AIC, added reduced excreta sheet
</commit_message>
<xml_diff>
--- a/Cummulative_Excretion.xlsx
+++ b/Cummulative_Excretion.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vassi\Documents\LAB\Genetic Algo\Data\Xie et al.2011\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptsir\Documents\GitHub\PBPK_Genetic_Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19136D1E-DA04-4406-9DAA-FCBA649E6F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cummulative_Excretion" sheetId="1" r:id="rId1"/>
+    <sheet name="reduced" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t xml:space="preserve">Time </t>
   </si>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -868,16 +868,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.983085774768931</v>
       </c>
@@ -899,7 +899,7 @@
         <v>16.150310160478</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2.03479323805665</v>
       </c>
@@ -910,7 +910,7 @@
         <v>21.3168179806434</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3.01345316682161</v>
       </c>
@@ -921,7 +921,7 @@
         <v>23.901371543918099</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4.0415139671737998</v>
       </c>
@@ -932,7 +932,7 @@
         <v>25.763036926542501</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4.9953470074021702</v>
       </c>
@@ -943,7 +943,7 @@
         <v>28.037851521062802</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5.9740069361671297</v>
       </c>
@@ -954,7 +954,7 @@
         <v>29.641342553455601</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7.0018991328620199</v>
       </c>
@@ -965,7 +965,7 @@
         <v>31.296608958942599</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7.9563222858909199</v>
       </c>
@@ -976,7 +976,7 @@
         <v>32.590290771057298</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8.9595561977065206</v>
       </c>
@@ -987,7 +987,7 @@
         <v>33.574233614417501</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9.9875326962300708</v>
       </c>
@@ -998,7 +998,7 @@
         <v>34.454906717684999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10.9907666080457</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>35.335579820952198</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11.945864175703701</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>35.854668330847403</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12.974009277884599</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>36.425672716884101</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13.929022543714</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>36.893337111304099</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15.0060627065102</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>37.309155881106697</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15.9119280062383</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>37.725044902432103</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17.062858721843799</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>38.037804686713599</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17.968808323400498</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>38.505398829609597</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18.972716649845299</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>38.714748370750002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20.001114657512101</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>39.130777895123401</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20.956127923341501</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>39.340127436264602</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21.935546568564298</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>39.549617480452604</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22.988602861110401</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>39.759107524641003</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23.967852902675901</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>40.071656554350199</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24.947440151555899</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>40.074536866828801</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25.9758381592227</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>40.490425888155002</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26.9063617438302</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>40.493306200633597</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27.934928355154199</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>40.651091123251902</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28.9634106646497</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>40.757241175823602</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29.967487594751699</v>
       </c>
@@ -1215,6 +1215,87 @@
         <v>7.5072651784273701</v>
       </c>
       <c r="C31">
+        <v>40.760121488301898</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.983085774768931</v>
+      </c>
+      <c r="B2">
+        <v>0.45337991789960502</v>
+      </c>
+      <c r="C2">
+        <v>16.150310160478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3.01345316682161</v>
+      </c>
+      <c r="B3">
+        <v>1.85335228563365</v>
+      </c>
+      <c r="C3">
+        <v>23.901371543918099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7.0018991328620199</v>
+      </c>
+      <c r="B4">
+        <v>3.9301980858800798</v>
+      </c>
+      <c r="C4">
+        <v>31.296608958942599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>15.0060627065102</v>
+      </c>
+      <c r="B5">
+        <v>6.3800092263668402</v>
+      </c>
+      <c r="C5">
+        <v>37.309155881106697</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>29.967487594751699</v>
+      </c>
+      <c r="B6">
+        <v>7.5072651784273701</v>
+      </c>
+      <c r="C6">
         <v>40.760121488301898</v>
       </c>
     </row>

</xml_diff>